<commit_message>
fix line breaks manually
</commit_message>
<xml_diff>
--- a/data/derived/list_medical_products.xlsx
+++ b/data/derived/list_medical_products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Dropbox/China Group Customs/_Aid/data_external/medical_products/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Projects/helble-medical-products/data/derived/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D713F14-5136-3148-872D-86D5C2F467F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674C7C45-A368-1042-A8DB-F3FC8028BD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-7120" windowWidth="25600" windowHeight="21100" xr2:uid="{8C33CDB8-57EA-234B-911D-3595F3C457BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{8C33CDB8-57EA-234B-911D-3595F3C457BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="217">
   <si>
     <t xml:space="preserve">Nr </t>
   </si>
   <si>
-    <t xml:space="preserve">HS Code  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 digit </t>
-  </si>
-  <si>
     <t xml:space="preserve">Group </t>
   </si>
   <si>
@@ -315,12 +309,6 @@
     <t xml:space="preserve">Polyphenols and phenol-alcohols (excl. resorcinol and hydroquinone "quinol" and their salts, and 4,4''-isopropylidenediphenol "bisphenol A, diphenylolpropane" and its salts) </t>
   </si>
   <si>
-    <t xml:space="preserve">Acyclic ethers and their halogenated, sulphonated, nitrated or nitrosated derivatives (excl. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">diethyl ether) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Aromatic ethers and their halogenated, sulphonated, nitrated or nitrosated derivatives </t>
   </si>
   <si>
@@ -480,12 +468,6 @@
     <t xml:space="preserve">Heterocyclic compounds with nitrogen hetero-atom[s] only, containing an unfused imidazole ring, whether or not hydrogenated, in the structure (excl. hydantoin and its derivatives) </t>
   </si>
   <si>
-    <t xml:space="preserve">Heterocyclic compounds with nitrogen hetero-atom[s] only, containing a pyrimidine ring, whether or not hydrogenated, or piperazine ring in the structure (excl. malonylurea </t>
-  </si>
-  <si>
-    <t xml:space="preserve">"barbituric acid" and its derivatives, allobarbital "INN", amobarbital "INN", barbital "INN", butalbital "INN", butobarbital "INN", cyclobarbital "INN", methylphenobarbital "INN", pentobarbital "INN", phenobarbital "INN", secbutabarbital "INN", secobarbital "INN", vinylbital "INN", loprazolam "INN", mecloqualone "INN", methaqualone "INN" and zipeprol "INN", and salts thereof) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Heterocyclic compounds with nitrogen hetero-atom[s] only, containing an unfused triazine ring, whether or not hydrogenated, in the structure (excl. melamine) </t>
   </si>
   <si>
@@ -498,12 +480,6 @@
     <t xml:space="preserve">Separate chemically defined organic compounds, n.e.s. </t>
   </si>
   <si>
-    <t xml:space="preserve">Colouring matter of vegetable or animal origin, incl. dye extracts (excl. animal black), whether or not chemically defined; preparations based on colouring matter of vegetable or animal origin of a kind used to dye fabrics or produce colorant preparations (excl. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">preparations of heading 3207, 3208, 3209, 3210, 3213 and 3215) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Synthetic organic colouring matter (excl. disperse dyes, acid dyes, mordant dyes, basic dyes, direct dyes, vat dyes and reactive dyes and organic pigments); preparations of the kind used for colouring any materials or for the production of prepared colours, based thereon (excl. preparations in heading 3207, 3208, 3209, 3210, 3212, 3213 and 3215); mixtures of colouring matter in subheading 3204.11 to 3204.19 </t>
   </si>
   <si>
@@ -600,12 +576,6 @@
     <t xml:space="preserve">Carriages for disabled persons, not mechanically propelled </t>
   </si>
   <si>
-    <t xml:space="preserve">Carriages for disabled persons, motorised or otherwise mechanically propelled (excl. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">specially designed motor vehicles and bicycles) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Cameras specially designed for underwater use, for aerial survey or for medical or surgical examination of internal organs; comparison cameras for forensic or criminological laboratories </t>
   </si>
   <si>
@@ -691,6 +661,21 @@
   </si>
   <si>
     <t xml:space="preserve">Operating tables, examination tables, and other medical, dental, surgical or veterinary furniture (excl. dentists'' or similar chairs, special tables for X-ray examination, and stretchers and litters, incl. trolley-stretchers) </t>
+  </si>
+  <si>
+    <t>HS Code  6 digit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acyclic ethers and their halogenated, sulphonated, nitrated or nitrosated derivatives (excl. diethyl ether) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heterocyclic compounds with nitrogen hetero-atom[s] only, containing a pyrimidine ring, whether or not hydrogenated, or piperazine ring in the structure (excl. malonylurea "barbituric acid" and its derivatives, allobarbital "INN", amobarbital "INN", barbital "INN", butalbital "INN", butobarbital "INN", cyclobarbital "INN", methylphenobarbital "INN", pentobarbital "INN", phenobarbital "INN", secbutabarbital "INN", secobarbital "INN", vinylbital "INN", loprazolam "INN", mecloqualone "INN", methaqualone "INN" and zipeprol "INN", and salts thereof) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colouring matter of vegetable or animal origin, incl. dye extracts (excl. animal black), whether or not chemically defined; preparations based on colouring matter of vegetable or animal origin of a kind used to dye fabrics or produce colorant preparations (excl. preparations of heading 3207, 3208, 3209, 3210, 3213 and 3215) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carriages for disabled persons, motorised or otherwise mechanically propelled (excl. specially designed motor vehicles and bicycles) </t>
   </si>
 </sst>
 </file>
@@ -1042,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92BF9EE-C94E-2647-81EC-FF7339F5A6B1}">
-  <dimension ref="A1:E219"/>
+  <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,3560 +1043,3535 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>300220</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>300220</v>
+        <v>300410</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>300410</v>
+        <v>300420</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>300420</v>
+        <v>300431</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>300432</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>300431</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>300432</v>
+        <v>300439</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>300439</v>
+        <v>300440</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>300440</v>
+        <v>300450</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>300450</v>
+        <v>300490</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>300490</v>
+        <v>300310</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>300310</v>
+        <v>300320</v>
       </c>
       <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>300320</v>
+        <v>300331</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>300331</v>
+        <v>300339</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>300339</v>
+        <v>300340</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>300340</v>
+        <v>300390</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>300660</v>
+      </c>
+      <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>300390</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>300660</v>
+        <v>293610</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>293610</v>
+        <v>293621</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
         <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>293621</v>
+        <v>293622</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>293622</v>
+        <v>293623</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>293623</v>
+        <v>293624</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>293624</v>
+        <v>293625</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>293626</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
         <v>31</v>
       </c>
-      <c r="E23" t="s">
-        <v>8</v>
+      <c r="E24" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>293625</v>
+        <v>293627</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
         <v>32</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>293626</v>
+        <v>293628</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>293627</v>
+        <v>293629</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
         <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>293628</v>
+        <v>293690</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>293629</v>
+        <v>293710</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" t="s">
         <v>36</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>293690</v>
+        <v>293711</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
         <v>37</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <v>293710</v>
+        <v>293712</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
         <v>38</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32">
-        <v>293711</v>
+        <v>293719</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33">
-        <v>293712</v>
+        <v>293721</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
         <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B34">
-        <v>293719</v>
+        <v>293722</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
         <v>41</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B35">
-        <v>293721</v>
+        <v>293723</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B36">
-        <v>293722</v>
+        <v>293729</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D36" t="s">
         <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B37">
-        <v>293723</v>
+        <v>293731</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D37" t="s">
         <v>44</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B38">
-        <v>293729</v>
+        <v>293739</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
         <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B39">
-        <v>293731</v>
+        <v>293740</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
         <v>46</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <v>293739</v>
+        <v>293750</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
         <v>47</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B41">
-        <v>293740</v>
+        <v>293790</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
         <v>48</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B42">
-        <v>293750</v>
+        <v>293791</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D42" t="s">
         <v>49</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B43">
-        <v>293790</v>
+        <v>293792</v>
       </c>
       <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" t="s">
         <v>25</v>
-      </c>
-      <c r="D43" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B44">
-        <v>293791</v>
+        <v>293799</v>
       </c>
       <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" t="s">
         <v>25</v>
-      </c>
-      <c r="D44" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B45">
-        <v>293792</v>
+        <v>293910</v>
       </c>
       <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" t="s">
         <v>25</v>
-      </c>
-      <c r="D45" t="s">
-        <v>44</v>
-      </c>
-      <c r="E45" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B46">
-        <v>293799</v>
+        <v>293911</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B47">
-        <v>293910</v>
+        <v>293919</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
         <v>53</v>
       </c>
       <c r="E47" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B48">
-        <v>293911</v>
+        <v>293920</v>
       </c>
       <c r="C48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D48" t="s">
         <v>54</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B49">
-        <v>293919</v>
+        <v>293921</v>
       </c>
       <c r="C49" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D49" t="s">
         <v>55</v>
       </c>
       <c r="E49" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B50">
-        <v>293920</v>
+        <v>293929</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D50" t="s">
         <v>56</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B51">
-        <v>293921</v>
+        <v>293930</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D51" t="s">
         <v>57</v>
       </c>
       <c r="E51" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B52">
-        <v>293929</v>
+        <v>293940</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D52" t="s">
         <v>58</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B53">
-        <v>293930</v>
+        <v>293941</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D53" t="s">
         <v>59</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B54">
-        <v>293940</v>
+        <v>293942</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
         <v>60</v>
       </c>
       <c r="E54" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B55">
-        <v>293941</v>
+        <v>293943</v>
       </c>
       <c r="C55" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D55" t="s">
         <v>61</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B56">
-        <v>293942</v>
+        <v>293949</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D56" t="s">
         <v>62</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>293950</v>
+      </c>
+      <c r="C57" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B58">
-        <v>293943</v>
+        <v>293951</v>
       </c>
       <c r="C58" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D58" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E58" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B59">
-        <v>293949</v>
+        <v>293959</v>
       </c>
       <c r="C59" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D59" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B60">
-        <v>293950</v>
+        <v>293960</v>
       </c>
       <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" t="s">
+        <v>66</v>
+      </c>
+      <c r="E60" t="s">
         <v>25</v>
-      </c>
-      <c r="D60" t="s">
-        <v>65</v>
-      </c>
-      <c r="E60" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B61">
-        <v>293951</v>
+        <v>293961</v>
       </c>
       <c r="C61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D61" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B62">
-        <v>293959</v>
+        <v>293962</v>
       </c>
       <c r="C62" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D62" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B63">
-        <v>293960</v>
+        <v>293963</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D63" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E63" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B64">
-        <v>293961</v>
+        <v>293969</v>
       </c>
       <c r="C64" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D64" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E64" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B65">
-        <v>293962</v>
+        <v>293970</v>
       </c>
       <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" t="s">
         <v>25</v>
-      </c>
-      <c r="D65" t="s">
-        <v>70</v>
-      </c>
-      <c r="E65" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B66">
-        <v>293963</v>
+        <v>293990</v>
       </c>
       <c r="C66" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" t="s">
+        <v>72</v>
+      </c>
+      <c r="E66" t="s">
         <v>25</v>
-      </c>
-      <c r="D66" t="s">
-        <v>71</v>
-      </c>
-      <c r="E66" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B67">
-        <v>293969</v>
+        <v>293991</v>
       </c>
       <c r="C67" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D67" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E67" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B68">
-        <v>293970</v>
+        <v>293999</v>
       </c>
       <c r="C68" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E68" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B69">
-        <v>293990</v>
+        <v>294110</v>
       </c>
       <c r="C69" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D69" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E69" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B70">
-        <v>293991</v>
+        <v>294120</v>
       </c>
       <c r="C70" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D70" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E70" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B71">
-        <v>293999</v>
+        <v>294130</v>
       </c>
       <c r="C71" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D71" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E71" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B72">
-        <v>294110</v>
+        <v>294140</v>
       </c>
       <c r="C72" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D72" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E72" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B73">
-        <v>294120</v>
+        <v>294150</v>
       </c>
       <c r="C73" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D73" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B74">
-        <v>294130</v>
+        <v>294190</v>
       </c>
       <c r="C74" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D74" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E74" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B75">
-        <v>294140</v>
+        <v>284210</v>
       </c>
       <c r="C75" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D75" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E75" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B76">
-        <v>294150</v>
+        <v>284290</v>
       </c>
       <c r="C76" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D76" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E76" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B77">
-        <v>294190</v>
+        <v>290290</v>
       </c>
       <c r="C77" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D77" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E77" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B78">
-        <v>284210</v>
+        <v>290349</v>
       </c>
       <c r="C78" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D78" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E78" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B79">
-        <v>284290</v>
+        <v>290369</v>
       </c>
       <c r="C79" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D79" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E79" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B80">
-        <v>290290</v>
+        <v>290410</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D80" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E80" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B81">
-        <v>290349</v>
+        <v>290490</v>
       </c>
       <c r="C81" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D81" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E81" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B82">
-        <v>290369</v>
+        <v>290522</v>
       </c>
       <c r="C82" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E82" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B83">
-        <v>290410</v>
+        <v>290529</v>
       </c>
       <c r="C83" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D83" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E83" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B84">
-        <v>290490</v>
+        <v>290619</v>
       </c>
       <c r="C84" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D84" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E84" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B85">
-        <v>290522</v>
+        <v>290629</v>
       </c>
       <c r="C85" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D85" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E85" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B86">
-        <v>290529</v>
+        <v>290729</v>
       </c>
       <c r="C86" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D86" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E86" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B87">
-        <v>290619</v>
+        <v>290919</v>
       </c>
       <c r="C87" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D87" t="s">
-        <v>93</v>
+        <v>213</v>
       </c>
       <c r="E87" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B88">
-        <v>290629</v>
+        <v>290930</v>
       </c>
       <c r="C88" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D88" t="s">
         <v>94</v>
       </c>
       <c r="E88" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>290949</v>
+      </c>
+      <c r="C89" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" t="s">
+        <v>95</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B90">
-        <v>290729</v>
+        <v>290950</v>
       </c>
       <c r="C90" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D90" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E90" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B91">
-        <v>290919</v>
+        <v>291229</v>
       </c>
       <c r="C91" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D91" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E91" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>291249</v>
+      </c>
+      <c r="C92" t="s">
+        <v>81</v>
+      </c>
       <c r="D92" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="E92" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B93">
-        <v>290930</v>
+        <v>291419</v>
       </c>
       <c r="C93" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D93" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E93" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B94">
-        <v>290949</v>
+        <v>291440</v>
       </c>
       <c r="C94" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D94" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E94" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B95">
-        <v>290950</v>
+        <v>291469</v>
       </c>
       <c r="C95" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D95" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E95" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B96">
-        <v>291229</v>
+        <v>291539</v>
       </c>
       <c r="C96" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D96" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E96" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B97">
-        <v>291249</v>
+        <v>291550</v>
       </c>
       <c r="C97" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D97" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E97" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B98">
-        <v>291419</v>
+        <v>291590</v>
       </c>
       <c r="C98" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D98" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E98" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B99">
-        <v>291440</v>
+        <v>291619</v>
       </c>
       <c r="C99" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D99" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E99" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B100">
-        <v>291469</v>
+        <v>291620</v>
       </c>
       <c r="C100" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D100" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E100" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B101">
-        <v>291539</v>
+        <v>291639</v>
       </c>
       <c r="C101" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D101" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E101" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B102">
-        <v>291550</v>
+        <v>291713</v>
       </c>
       <c r="C102" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D102" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E102" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B103">
-        <v>291590</v>
+        <v>291719</v>
       </c>
       <c r="C103" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D103" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E103" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B104">
-        <v>291619</v>
+        <v>291734</v>
       </c>
       <c r="C104" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D104" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E104" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B105">
-        <v>291620</v>
+        <v>291739</v>
       </c>
       <c r="C105" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D105" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E105" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B106">
-        <v>291639</v>
+        <v>291811</v>
       </c>
       <c r="C106" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D106" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E106" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B107">
-        <v>291713</v>
+        <v>291813</v>
       </c>
       <c r="C107" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D107" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E107" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B108">
-        <v>291719</v>
+        <v>291816</v>
       </c>
       <c r="C108" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D108" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E108" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B109">
-        <v>291734</v>
+        <v>291819</v>
       </c>
       <c r="C109" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D109" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E109" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B110">
-        <v>291739</v>
+        <v>291822</v>
       </c>
       <c r="C110" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D110" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E110" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B111">
-        <v>291811</v>
+        <v>291823</v>
       </c>
       <c r="C111" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D111" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E111" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B112">
-        <v>291813</v>
+        <v>291829</v>
       </c>
       <c r="C112" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D112" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E112" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B113">
-        <v>291816</v>
+        <v>291830</v>
       </c>
       <c r="C113" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D113" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E113" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B114">
-        <v>291819</v>
+        <v>292090</v>
       </c>
       <c r="C114" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D114" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E114" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B115">
-        <v>291822</v>
+        <v>292119</v>
       </c>
       <c r="C115" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D115" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E115" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B116">
-        <v>291823</v>
+        <v>292129</v>
       </c>
       <c r="C116" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D116" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E116" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B117">
-        <v>291829</v>
+        <v>292130</v>
       </c>
       <c r="C117" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D117" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E117" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>292142</v>
+      </c>
+      <c r="C118" t="s">
+        <v>81</v>
+      </c>
+      <c r="D118" t="s">
+        <v>124</v>
+      </c>
+      <c r="E118" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B119">
-        <v>291830</v>
+        <v>292149</v>
       </c>
       <c r="C119" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D119" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E119" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B120">
-        <v>292090</v>
+        <v>292159</v>
       </c>
       <c r="C120" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D120" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E120" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B121">
-        <v>292119</v>
+        <v>292211</v>
       </c>
       <c r="C121" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D121" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E121" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B122">
-        <v>292129</v>
+        <v>292219</v>
       </c>
       <c r="C122" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D122" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E122" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B123">
-        <v>292130</v>
+        <v>292229</v>
       </c>
       <c r="C123" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D123" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E123" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B124">
-        <v>292142</v>
+        <v>292241</v>
       </c>
       <c r="C124" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D124" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E124" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B125">
-        <v>292149</v>
+        <v>292249</v>
       </c>
       <c r="C125" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D125" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E125" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B126">
-        <v>292159</v>
+        <v>292250</v>
       </c>
       <c r="C126" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D126" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E126" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B127">
-        <v>292211</v>
+        <v>292310</v>
       </c>
       <c r="C127" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D127" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E127" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B128">
-        <v>292219</v>
+        <v>292390</v>
       </c>
       <c r="C128" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D128" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E128" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B129">
-        <v>292229</v>
+        <v>292429</v>
       </c>
       <c r="C129" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D129" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E129" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B130">
-        <v>292241</v>
+        <v>292519</v>
       </c>
       <c r="C130" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D130" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E130" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B131">
-        <v>292249</v>
+        <v>292690</v>
       </c>
       <c r="C131" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D131" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E131" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B132">
-        <v>292250</v>
+        <v>292700</v>
       </c>
       <c r="C132" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D132" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E132" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B133">
-        <v>292310</v>
+        <v>292800</v>
       </c>
       <c r="C133" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D133" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E133" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B134">
-        <v>292390</v>
+        <v>292990</v>
       </c>
       <c r="C134" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D134" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E134" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B135">
-        <v>292429</v>
+        <v>293090</v>
       </c>
       <c r="C135" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D135" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E135" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B136">
-        <v>292519</v>
+        <v>293100</v>
       </c>
       <c r="C136" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D136" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E136" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B137">
-        <v>292690</v>
+        <v>293299</v>
       </c>
       <c r="C137" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D137" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E137" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B138">
-        <v>292700</v>
+        <v>293311</v>
       </c>
       <c r="C138" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D138" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E138" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B139">
-        <v>292800</v>
+        <v>293321</v>
       </c>
       <c r="C139" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D139" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E139" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B140">
-        <v>292990</v>
+        <v>293329</v>
       </c>
       <c r="C140" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D140" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E140" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B141">
-        <v>293090</v>
+        <v>293359</v>
       </c>
       <c r="C141" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D141" t="s">
-        <v>145</v>
+        <v>214</v>
       </c>
       <c r="E141" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B142">
-        <v>293100</v>
+        <v>293369</v>
       </c>
       <c r="C142" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D142" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E142" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>293810</v>
+      </c>
+      <c r="C143" t="s">
+        <v>81</v>
+      </c>
+      <c r="D143" t="s">
+        <v>148</v>
+      </c>
+      <c r="E143" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B144">
-        <v>293299</v>
+        <v>294000</v>
       </c>
       <c r="C144" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D144" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E144" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B145">
-        <v>293311</v>
+        <v>294200</v>
       </c>
       <c r="C145" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D145" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E145" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B146">
-        <v>293321</v>
+        <v>320300</v>
       </c>
       <c r="C146" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D146" t="s">
-        <v>149</v>
+        <v>215</v>
       </c>
       <c r="E146" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B147">
-        <v>293329</v>
+        <v>320419</v>
       </c>
       <c r="C147" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D147" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E147" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B148">
-        <v>293359</v>
+        <v>293890</v>
       </c>
       <c r="C148" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="D148" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E148" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>300110</v>
+      </c>
+      <c r="C149" t="s">
+        <v>152</v>
+      </c>
       <c r="D149" t="s">
-        <v>152</v>
+        <v>154</v>
+      </c>
+      <c r="E149" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B150">
-        <v>293369</v>
+        <v>300120</v>
       </c>
       <c r="C150" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="D150" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E150" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B151">
-        <v>293810</v>
+        <v>300190</v>
       </c>
       <c r="C151" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="D151" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E151" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B152">
-        <v>294000</v>
+        <v>300210</v>
       </c>
       <c r="C152" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="D152" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E152" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B153">
-        <v>294200</v>
+        <v>300290</v>
       </c>
       <c r="C153" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="D153" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E153" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B154">
-        <v>320300</v>
+        <v>300510</v>
       </c>
       <c r="C154" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="D154" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E154" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155">
+        <v>300590</v>
+      </c>
+      <c r="C155" t="s">
+        <v>152</v>
+      </c>
       <c r="D155" t="s">
-        <v>158</v>
+        <v>160</v>
+      </c>
+      <c r="E155" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B156">
-        <v>320419</v>
+        <v>300610</v>
       </c>
       <c r="C156" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="D156" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E156" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B157">
-        <v>293890</v>
+        <v>300620</v>
       </c>
       <c r="C157" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D157" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E157" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="B158">
-        <v>300110</v>
+        <v>300630</v>
       </c>
       <c r="C158" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D158" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E158" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B159">
-        <v>300120</v>
+        <v>300640</v>
       </c>
       <c r="C159" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D159" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E159" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B160">
-        <v>300190</v>
+        <v>300650</v>
       </c>
       <c r="C160" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D160" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E160" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B161">
-        <v>300210</v>
+        <v>300670</v>
       </c>
       <c r="C161" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D161" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E161" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162">
+        <v>300680</v>
+      </c>
+      <c r="C162" t="s">
         <v>152</v>
       </c>
-      <c r="B162">
-        <v>300290</v>
-      </c>
-      <c r="C162" t="s">
-        <v>160</v>
-      </c>
       <c r="D162" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E162" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B163">
-        <v>300510</v>
+        <v>300691</v>
       </c>
       <c r="C163" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D163" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E163" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B164">
-        <v>300590</v>
+        <v>300692</v>
       </c>
       <c r="C164" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D164" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E164" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B165">
-        <v>300610</v>
+        <v>350790</v>
       </c>
       <c r="C165" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D165" t="s">
         <v>169</v>
       </c>
       <c r="E165" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B166">
-        <v>300620</v>
+        <v>382200</v>
       </c>
       <c r="C166" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D166" t="s">
         <v>170</v>
       </c>
       <c r="E166" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B167">
-        <v>300630</v>
+        <v>382490</v>
       </c>
       <c r="C167" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D167" t="s">
         <v>171</v>
       </c>
       <c r="E167" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168">
+        <v>401490</v>
+      </c>
+      <c r="C168" t="s">
+        <v>152</v>
+      </c>
+      <c r="D168" t="s">
+        <v>172</v>
+      </c>
+      <c r="E168" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="B169">
-        <v>300640</v>
+        <v>401511</v>
       </c>
       <c r="C169" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D169" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E169" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B170">
-        <v>300650</v>
+        <v>701710</v>
       </c>
       <c r="C170" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D170" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E170" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B171">
-        <v>300670</v>
+        <v>701720</v>
       </c>
       <c r="C171" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D171" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E171" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B172">
-        <v>300680</v>
+        <v>701790</v>
       </c>
       <c r="C172" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D172" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E172" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B173">
-        <v>300691</v>
+        <v>901831</v>
       </c>
       <c r="C173" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D173" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E173" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B174">
-        <v>300692</v>
+        <v>901832</v>
       </c>
       <c r="C174" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D174" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E174" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B175">
-        <v>350790</v>
+        <v>901839</v>
       </c>
       <c r="C175" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D175" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E175" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B176">
-        <v>382200</v>
+        <v>841920</v>
       </c>
       <c r="C176" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D176" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E176" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="B177">
-        <v>382490</v>
+        <v>871310</v>
       </c>
       <c r="C177" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D177" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E177" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B178">
-        <v>401490</v>
+        <v>871390</v>
       </c>
       <c r="C178" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D178" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
       <c r="E178" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B179">
-        <v>401511</v>
+        <v>900630</v>
       </c>
       <c r="C179" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D179" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E179" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B180">
-        <v>701710</v>
+        <v>901811</v>
       </c>
       <c r="C180" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D180" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E180" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B181">
-        <v>701720</v>
+        <v>901812</v>
       </c>
       <c r="C181" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D181" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E181" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B182">
-        <v>701790</v>
+        <v>901813</v>
       </c>
       <c r="C182" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D182" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E182" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="B183">
-        <v>901831</v>
+        <v>901814</v>
       </c>
       <c r="C183" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D183" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E183" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="B184">
-        <v>901832</v>
+        <v>901819</v>
       </c>
       <c r="C184" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D184" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E184" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="B185">
-        <v>901839</v>
+        <v>901820</v>
       </c>
       <c r="C185" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D185" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E185" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B186">
-        <v>841920</v>
+        <v>901841</v>
       </c>
       <c r="C186" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D186" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E186" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B187">
-        <v>871310</v>
+        <v>901849</v>
       </c>
       <c r="C187" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D187" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E187" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B188">
-        <v>871390</v>
+        <v>901850</v>
       </c>
       <c r="C188" t="s">
+        <v>180</v>
+      </c>
+      <c r="D188" t="s">
+        <v>192</v>
+      </c>
+      <c r="E188" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189">
         <v>188</v>
       </c>
-      <c r="D188" t="s">
-        <v>191</v>
-      </c>
-      <c r="E188" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B189">
+        <v>901890</v>
+      </c>
+      <c r="C189" t="s">
+        <v>180</v>
+      </c>
       <c r="D189" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="E189" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B190">
-        <v>900630</v>
+        <v>901920</v>
       </c>
       <c r="C190" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D190" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E190" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="B191">
-        <v>901811</v>
+        <v>902110</v>
       </c>
       <c r="C191" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D191" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E191" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192">
+        <v>902111</v>
+      </c>
+      <c r="C192" t="s">
         <v>180</v>
       </c>
-      <c r="B192">
-        <v>901812</v>
-      </c>
-      <c r="C192" t="s">
-        <v>188</v>
-      </c>
       <c r="D192" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E192" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="B193">
-        <v>901813</v>
+        <v>902119</v>
       </c>
       <c r="C193" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D193" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E193" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="B194">
-        <v>901814</v>
+        <v>902121</v>
       </c>
       <c r="C194" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D194" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E194" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="B195">
-        <v>901819</v>
+        <v>902129</v>
       </c>
       <c r="C195" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D195" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E195" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B196">
-        <v>901820</v>
+        <v>902130</v>
       </c>
       <c r="C196" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D196" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E196" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="B197">
-        <v>901841</v>
+        <v>902131</v>
       </c>
       <c r="C197" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D197" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E197" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B198">
-        <v>901849</v>
+        <v>902139</v>
       </c>
       <c r="C198" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D198" t="s">
         <v>201</v>
       </c>
       <c r="E198" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="B199">
-        <v>901850</v>
+        <v>902140</v>
       </c>
       <c r="C199" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D199" t="s">
         <v>202</v>
       </c>
       <c r="E199" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B200">
-        <v>901890</v>
+        <v>902150</v>
       </c>
       <c r="C200" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D200" t="s">
         <v>203</v>
       </c>
       <c r="E200" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="B201">
-        <v>901920</v>
+        <v>902190</v>
       </c>
       <c r="C201" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D201" t="s">
         <v>204</v>
       </c>
       <c r="E201" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B202">
-        <v>902110</v>
+        <v>902211</v>
       </c>
       <c r="C202" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D202" t="s">
         <v>205</v>
       </c>
       <c r="E202" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="B203">
-        <v>902111</v>
+        <v>902212</v>
       </c>
       <c r="C203" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D203" t="s">
         <v>206</v>
       </c>
       <c r="E203" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B204">
-        <v>902119</v>
+        <v>902213</v>
       </c>
       <c r="C204" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D204" t="s">
         <v>207</v>
       </c>
       <c r="E204" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B205">
-        <v>902121</v>
+        <v>902214</v>
       </c>
       <c r="C205" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D205" t="s">
         <v>208</v>
       </c>
       <c r="E205" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B206">
-        <v>902129</v>
+        <v>902221</v>
       </c>
       <c r="C206" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D206" t="s">
         <v>209</v>
       </c>
       <c r="E206" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B207">
-        <v>902130</v>
+        <v>940210</v>
       </c>
       <c r="C207" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D207" t="s">
         <v>210</v>
       </c>
       <c r="E207" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B208">
-        <v>902131</v>
+        <v>940290</v>
       </c>
       <c r="C208" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D208" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E208" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A209">
-        <v>197</v>
-      </c>
-      <c r="B209">
-        <v>902139</v>
-      </c>
-      <c r="C209" t="s">
-        <v>188</v>
-      </c>
-      <c r="D209" t="s">
-        <v>211</v>
-      </c>
-      <c r="E209" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A210">
-        <v>198</v>
-      </c>
-      <c r="B210">
-        <v>902140</v>
-      </c>
-      <c r="C210" t="s">
-        <v>188</v>
-      </c>
-      <c r="D210" t="s">
-        <v>212</v>
-      </c>
-      <c r="E210" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211">
-        <v>199</v>
-      </c>
-      <c r="B211">
-        <v>902150</v>
-      </c>
-      <c r="C211" t="s">
-        <v>188</v>
-      </c>
-      <c r="D211" t="s">
-        <v>213</v>
-      </c>
-      <c r="E211" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A212">
-        <v>200</v>
-      </c>
-      <c r="B212">
-        <v>902190</v>
-      </c>
-      <c r="C212" t="s">
-        <v>188</v>
-      </c>
-      <c r="D212" t="s">
-        <v>214</v>
-      </c>
-      <c r="E212" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213">
-        <v>201</v>
-      </c>
-      <c r="B213">
-        <v>902211</v>
-      </c>
-      <c r="C213" t="s">
-        <v>188</v>
-      </c>
-      <c r="D213" t="s">
-        <v>215</v>
-      </c>
-      <c r="E213" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214">
-        <v>202</v>
-      </c>
-      <c r="B214">
-        <v>902212</v>
-      </c>
-      <c r="C214" t="s">
-        <v>188</v>
-      </c>
-      <c r="D214" t="s">
-        <v>216</v>
-      </c>
-      <c r="E214" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A215">
-        <v>203</v>
-      </c>
-      <c r="B215">
-        <v>902213</v>
-      </c>
-      <c r="C215" t="s">
-        <v>188</v>
-      </c>
-      <c r="D215" t="s">
-        <v>217</v>
-      </c>
-      <c r="E215" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A216">
-        <v>204</v>
-      </c>
-      <c r="B216">
-        <v>902214</v>
-      </c>
-      <c r="C216" t="s">
-        <v>188</v>
-      </c>
-      <c r="D216" t="s">
-        <v>218</v>
-      </c>
-      <c r="E216" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A217">
-        <v>205</v>
-      </c>
-      <c r="B217">
-        <v>902221</v>
-      </c>
-      <c r="C217" t="s">
-        <v>188</v>
-      </c>
-      <c r="D217" t="s">
-        <v>219</v>
-      </c>
-      <c r="E217" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A218">
-        <v>206</v>
-      </c>
-      <c r="B218">
-        <v>940210</v>
-      </c>
-      <c r="C218" t="s">
-        <v>188</v>
-      </c>
-      <c r="D218" t="s">
-        <v>220</v>
-      </c>
-      <c r="E218" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A219">
-        <v>207</v>
-      </c>
-      <c r="B219">
-        <v>940290</v>
-      </c>
-      <c r="C219" t="s">
-        <v>188</v>
-      </c>
-      <c r="D219" t="s">
-        <v>221</v>
-      </c>
-      <c r="E219" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>